<commit_message>
Refactored code and cleaned up wiki
</commit_message>
<xml_diff>
--- a/other/results/Training Results.xlsx
+++ b/other/results/Training Results.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevond/Desktop/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevond/code/final-year-project/other/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53C2D1C-40AD-A540-B4D5-6D98FB1B4EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5458F286-6CDE-F641-AE51-E7B456345F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{603C461D-5AF7-E448-B1FF-80E0B3DBD308}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -217,9 +217,6 @@
     <t>Added data augmentation: Low mask frequency band.</t>
   </si>
   <si>
-    <t>Pretty much as the previous good one.</t>
-  </si>
-  <si>
     <t>Added data augmentation: Low noise</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Increasing number of epoches to 1000 and decreasing learning rate to 0.00005</t>
+  </si>
+  <si>
+    <t>Pretty much as the previous good one. Keeping this one due to lower loss.</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,7 +1063,7 @@
         <v>36</v>
       </c>
       <c r="Z5" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -1525,7 +1525,7 @@
         <v>0.96</v>
       </c>
       <c r="Z11" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -1978,7 +1978,7 @@
         <v>0.97</v>
       </c>
       <c r="Y17" s="18" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -2007,7 +2007,7 @@
         <v>14</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" s="17">
         <v>0.98499999999999999</v>
@@ -2055,7 +2055,7 @@
         <v>0.96</v>
       </c>
       <c r="Z18" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -2084,7 +2084,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J19" s="17">
         <v>0.9</v>

</xml_diff>

<commit_message>
Updated wiki and added Seq Diagram for Gateway Framework
</commit_message>
<xml_diff>
--- a/other/results/Training Results.xlsx
+++ b/other/results/Training Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruslanlevond/code/final-year-project/other/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5458F286-6CDE-F641-AE51-E7B456345F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFCDFC6-971C-DA4F-B044-E7BAC90954CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{603C461D-5AF7-E448-B1FF-80E0B3DBD308}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>Added data augmentation: Warp time axis</t>
   </si>
   <si>
-    <t>Added data augmentation: Low mask frequency band.</t>
-  </si>
-  <si>
     <t>Added data augmentation: Low noise</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Pretty much as the previous good one. Keeping this one due to lower loss.</t>
+  </si>
+  <si>
+    <t>Added data augmentation: Low mask time band.</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,7 +1063,7 @@
         <v>36</v>
       </c>
       <c r="Z5" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -1525,7 +1525,7 @@
         <v>0.96</v>
       </c>
       <c r="Z11" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -1930,7 +1930,7 @@
         <v>14</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="J17" s="19">
         <v>0.97699999999999998</v>
@@ -1978,7 +1978,7 @@
         <v>0.97</v>
       </c>
       <c r="Y17" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -2007,7 +2007,7 @@
         <v>14</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" s="17">
         <v>0.98499999999999999</v>
@@ -2055,7 +2055,7 @@
         <v>0.96</v>
       </c>
       <c r="Z18" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -2084,7 +2084,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" s="17">
         <v>0.9</v>

</xml_diff>